<commit_message>
[11.01.2020] Resolving comments and adding id check
</commit_message>
<xml_diff>
--- a/sheet1.xlsx
+++ b/sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannesschmid/Desktop/CodeBaking/Python Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3569430-9BE9-9843-9D47-CC0395D56090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1D6660-14E5-8640-BB49-4975D3418DE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9640" yWindow="520" windowWidth="28040" windowHeight="16120" xr2:uid="{0E65528D-4654-8147-BC20-CC3780B0CD56}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>